<commit_message>
Update design. -Add and update documents of design.
</commit_message>
<xml_diff>
--- a/dev/doc/hw_component_design.xlsx
+++ b/dev/doc/hw_component_design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22470" windowHeight="12945" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22470" windowHeight="12945"/>
   </bookViews>
   <sheets>
     <sheet name="基本" sheetId="2" r:id="rId1"/>
@@ -7104,7 +7104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10562,7 +10562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BW47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.28515625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>